<commit_message>
Minor changes to board layout.
</commit_message>
<xml_diff>
--- a/Clue Board Layout.xlsx
+++ b/Clue Board Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\hornet\Users\a\adamnelson\adit\My Documents\Eclipse Projects\Clue-CSCI-306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\Eclipse Projects\Clue-CSCI-306\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -483,7 +483,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1263,8 +1263,8 @@
       <c r="O12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>10</v>
+      <c r="P12" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="Q12" s="3" t="s">
         <v>10</v>
@@ -2081,11 +2081,11 @@
       <c r="F25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>16</v>
+      <c r="G25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>16</v>
@@ -2096,11 +2096,11 @@
       <c r="K25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="L25" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>16</v>
+      <c r="L25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="N25" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Added stubs for testing target cells
</commit_message>
<xml_diff>
--- a/Clue Board Layout.xlsx
+++ b/Clue Board Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\Eclipse Projects\Clue-CSCI-306\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\Eclipse Projects\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="29">
   <si>
     <t>K</t>
   </si>
@@ -93,6 +93,24 @@
   </si>
   <si>
     <t>RU</t>
+  </si>
+  <si>
+    <t>Door Direction Tests: White</t>
+  </si>
+  <si>
+    <t>Adjacency List Tests, Inside Room: Orange</t>
+  </si>
+  <si>
+    <t>Adjacency List Tests, Room Exits: Purple</t>
+  </si>
+  <si>
+    <t>Adjacency List Tests, beside Room Entrance: Green</t>
+  </si>
+  <si>
+    <t>Walkway Scenarios: Dark Red</t>
+  </si>
+  <si>
+    <t>Test Targets: Blue</t>
   </si>
 </sst>
 </file>
@@ -180,7 +198,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,6 +214,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -480,26 +501,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="2.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="3.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="2.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4" style="6" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="3" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -2187,6 +2208,37 @@
       </c>
       <c r="T26" s="1">
         <v>19</v>
+      </c>
+      <c r="U26" s="1"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Designated cells to test targets on
</commit_message>
<xml_diff>
--- a/Clue Board Layout.xlsx
+++ b/Clue Board Layout.xlsx
@@ -117,7 +117,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +153,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +189,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -192,13 +205,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,8 +232,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -503,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,7 +1207,7 @@
       <c r="E11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1751,7 +1769,7 @@
       <c r="S19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T19" s="2" t="s">
+      <c r="T19" s="7" t="s">
         <v>2</v>
       </c>
       <c r="U19" s="1">
@@ -2099,7 +2117,7 @@
       <c r="E25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="7" t="s">
         <v>2</v>
       </c>
       <c r="G25" s="2" t="s">

</xml_diff>

<commit_message>
Updated spreadsheet file with test tiles.
</commit_message>
<xml_diff>
--- a/Clue Board Layout.xlsx
+++ b/Clue Board Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\Eclipse Projects\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="31">
   <si>
     <t>K</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Test Targets: Blue</t>
+  </si>
+  <si>
+    <t>Adjacency List Tests, Board Edges: Brown</t>
+  </si>
+  <si>
+    <t>Adjacency List Tests, Room Edges: Grey</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,6 +201,42 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -212,7 +254,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,6 +275,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -519,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +626,7 @@
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -610,7 +676,7 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -684,7 +750,7 @@
       <c r="D3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -705,7 +771,7 @@
       <c r="K3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -714,7 +780,7 @@
       <c r="N3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="P3" s="3" t="s">
@@ -776,7 +842,7 @@
       <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="O4" s="4" t="s">
@@ -817,7 +883,7 @@
       <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="10" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -935,7 +1001,7 @@
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1045,7 +1111,7 @@
       <c r="P8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="12" t="s">
         <v>2</v>
       </c>
       <c r="R8" s="2" t="s">
@@ -1119,7 +1185,7 @@
       <c r="S9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="T9" s="14" t="s">
         <v>2</v>
       </c>
       <c r="U9" s="1">
@@ -1192,7 +1258,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1314,7 +1380,7 @@
       <c r="S12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="T12" s="3" t="s">
+      <c r="T12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="U12" s="1">
@@ -1402,7 +1468,7 @@
       <c r="E14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="15" t="s">
         <v>2</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1452,7 +1518,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1559,7 +1625,7 @@
       <c r="N16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" s="15" t="s">
         <v>2</v>
       </c>
       <c r="P16" s="3" t="s">
@@ -1585,7 +1651,7 @@
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="13" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1630,7 +1696,7 @@
       <c r="P17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q17" s="4" t="s">
+      <c r="Q17" s="13" t="s">
         <v>15</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -1893,7 +1959,7 @@
       <c r="Q21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="R21" s="8" t="s">
         <v>14</v>
       </c>
       <c r="S21" s="3" t="s">
@@ -1981,7 +2047,7 @@
       <c r="C23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -2049,7 +2115,7 @@
       <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="12" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="2" t="s">
@@ -2141,7 +2207,7 @@
       <c r="M25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="N25" s="14" t="s">
         <v>2</v>
       </c>
       <c r="O25" s="2" t="s">
@@ -2236,26 +2302,36 @@
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected error in cell color
</commit_message>
<xml_diff>
--- a/Clue Board Layout.xlsx
+++ b/Clue Board Layout.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\CSCI306\ClueGame\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\My Documents\Eclipse Projects\ClueGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -254,7 +254,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -299,6 +299,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -587,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +774,7 @@
       <c r="K3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="M3" s="2" t="s">
@@ -1959,7 +1962,7 @@
       <c r="Q21" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="R21" s="8" t="s">
+      <c r="R21" s="16" t="s">
         <v>14</v>
       </c>
       <c r="S21" s="3" t="s">

</xml_diff>

<commit_message>
Added cells with the name door directio modifier.
</commit_message>
<xml_diff>
--- a/Clue Board Layout.xlsx
+++ b/Clue Board Layout.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="39">
   <si>
     <t>K</t>
   </si>
@@ -117,6 +117,30 @@
   </si>
   <si>
     <t>Adjacency List Tests, Room Edges: Grey</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>AN</t>
+  </si>
+  <si>
+    <t>QN</t>
+  </si>
+  <si>
+    <t>LN</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>MN</t>
   </si>
 </sst>
 </file>
@@ -167,7 +191,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +261,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -247,14 +276,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,9 +334,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="40% - Accent1" xfId="4" builtinId="31"/>
+    <cellStyle name="Accent1" xfId="5" builtinId="29"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -590,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,8 +711,8 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
+      <c r="A2" s="17" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>0</v>
@@ -697,8 +732,8 @@
       <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>3</v>
+      <c r="H2" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>3</v>
@@ -718,8 +753,8 @@
       <c r="N2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>5</v>
+      <c r="O2" s="18" t="s">
+        <v>33</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>5</v>
@@ -1196,8 +1231,8 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
+      <c r="A10" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -1306,8 +1341,8 @@
       <c r="O11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P11" s="3" t="s">
-        <v>10</v>
+      <c r="P11" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>10</v>
@@ -1846,8 +1881,8 @@
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>18</v>
+      <c r="A20" s="18" t="s">
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>18</v>
@@ -2059,8 +2094,8 @@
       <c r="F23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>16</v>
+      <c r="G23" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>16</v>
@@ -2086,8 +2121,8 @@
       <c r="O23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="3" t="s">
-        <v>13</v>
+      <c r="P23" s="18" t="s">
+        <v>38</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>13</v>

</xml_diff>